<commit_message>
train and test data collection good
</commit_message>
<xml_diff>
--- a/HRI/Lab2_EMGInterfacing/FeatureData/DataLog.xlsx
+++ b/HRI/Lab2_EMGInterfacing/FeatureData/DataLog.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smithjl3\Documents\GitHub\HRI-LABS-BBALL\HRI\Lab2_EMGInterfacing\FeatureData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Documents\GitHub\HRI-LABS-BBALL\HRI\Lab2_EMGInterfacing\FeatureData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5224A0F2-F2CF-4EBE-BD5A-E24BC318C96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19770" yWindow="3225" windowWidth="7740" windowHeight="8640" xr2:uid="{46495FDF-836F-4063-8C47-2121ECC8C019}"/>
+    <workbookView xWindow="19770" yWindow="3225" windowWidth="7740" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,11 +389,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7B3DED-F1AD-4332-A2B4-430727191087}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +419,151 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>